<commit_message>
Task 1 just has a little change to a name. The excel file had repeat info that I deleted. Task 5 is just a start.
</commit_message>
<xml_diff>
--- a/FruitSoul Expected Delivery Costs and Times.xlsx
+++ b/FruitSoul Expected Delivery Costs and Times.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natej\OneDrive - Georgia Institute of Technology\ISYE6202 Fall 24 Warehouse Systems\(Old) Casework 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natej\OneDrive - Georgia Institute of Technology\ISYE6202 Fall 24 Warehouse Systems\Casework1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D09B389-E8DB-4037-AEB8-723B7321EE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D6BD3C-F200-46C5-8A60-4B7A660352C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Alabama</t>
   </si>
@@ -198,9 +198,6 @@
   </si>
   <si>
     <t>Destination State</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -693,7 +690,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,8 +846,8 @@
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>54</v>
+      <c r="B11" s="3">
+        <v>0</v>
       </c>
       <c r="C11" s="9">
         <v>0.90999999999999992</v>
@@ -1431,15 +1428,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007223C2B312D46944BF149C49909D2D6C" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bd4d5da4979e115853fe77acfdeaca0b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="283f4fa9-8f89-467f-bdab-4531434f2e70" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b7d3582f4974d32570ddc2d189cfa64" ns2:_="">
     <xsd:import namespace="283f4fa9-8f89-467f-bdab-4531434f2e70"/>
@@ -1583,6 +1571,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39A59016-65B6-4747-BC2E-22ACA402C965}">
   <ds:schemaRefs>
@@ -1600,14 +1597,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86EB2231-B970-4647-A0C9-66DBE3833C6E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{471E4E93-28BD-4E4D-ACE1-8E3C6B1C6D5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1623,4 +1612,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86EB2231-B970-4647-A0C9-66DBE3833C6E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>